<commit_message>
pruebas 1-5 + actualizacion reparto excel
</commit_message>
<xml_diff>
--- a/Trabajo dia 31/Reparto de simulaciones.xlsx
+++ b/Trabajo dia 31/Reparto de simulaciones.xlsx
@@ -5,33 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\uni\MCG\ARENA\Trabajo Grupo\trunk\Trabajo dia 31\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hornet\Documents\MCG\Trabajo dia 31\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A577AA6-4951-4E84-B331-5BBFA29DA3D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7534CC98-1DB5-4FE0-BE28-9845232D2FFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8412" xr2:uid="{76F68D2D-71FF-438A-AB09-9328E271E120}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8415" xr2:uid="{76F68D2D-71FF-438A-AB09-9328E271E120}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="8">
   <si>
     <t>Herramientas</t>
   </si>
@@ -115,7 +109,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,16 +484,16 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="7" t="s">
         <v>0</v>
@@ -509,7 +503,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2">
         <v>1</v>
@@ -527,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -550,98 +544,110 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
         <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>3</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>3</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
         <v>2</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
       <c r="C9" s="5">
         <v>2</v>
       </c>
@@ -658,8 +664,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>7</v>
+      </c>
       <c r="C10" s="5">
         <v>2</v>
       </c>
@@ -676,8 +684,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>8</v>
+      </c>
       <c r="C11" s="5">
         <v>2</v>
       </c>
@@ -694,8 +704,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
       <c r="C12" s="5">
         <v>2</v>
       </c>
@@ -712,8 +724,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
       <c r="C13" s="5">
         <v>2</v>
       </c>
@@ -730,8 +744,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>11</v>
+      </c>
       <c r="C14" s="5">
         <v>2</v>
       </c>
@@ -748,108 +764,120 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="5">
-        <v>3</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
         <v>1</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="5">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
         <v>2</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="5">
-        <v>3</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2</v>
-      </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8">
+        <v>3</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8">
         <v>1</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="5">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>15</v>
+      </c>
+      <c r="C18" s="8">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
         <v>2</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="5">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5">
-        <v>3</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8">
+        <v>3</v>
+      </c>
+      <c r="D19" s="8">
+        <v>3</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
         <v>1</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="5">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" s="5">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>17</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3</v>
+      </c>
+      <c r="D20" s="8">
+        <v>3</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8">
         <v>2</v>
       </c>
       <c r="G20" s="6" t="s">

</xml_diff>